<commit_message>
updated BOM with shoulder
</commit_message>
<xml_diff>
--- a/Documents/TB_BOM.xlsx
+++ b/Documents/TB_BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trott\Documents\UofSC-ASME-Tiger-Burn-Design-2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Win\Documents\GitHub\UofSC-ASME-Tiger-Burn-Design-2025\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC736C8E-3DDD-403C-867A-D2C422249834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6573D5E0-20B7-4022-BA13-464722788A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-930" windowWidth="29040" windowHeight="17520" xr2:uid="{5E11D219-2DD1-4F5F-BD59-159B1B8915B2}"/>
+    <workbookView xWindow="5016" yWindow="1644" windowWidth="23040" windowHeight="12216" xr2:uid="{5E11D219-2DD1-4F5F-BD59-159B1B8915B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Wood lengths</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>4x4x192</t>
+  </si>
+  <si>
+    <t>Front Shoulder</t>
   </si>
 </sst>
 </file>
@@ -553,34 +556,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FB1068-2A37-45DD-A633-D1C139FB0473}">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.28515625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.5546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.33203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="5.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,31 +607,34 @@
         <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -650,38 +657,41 @@
         <v>3</v>
       </c>
       <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4">
         <f>6+0.5+1+1+1</f>
         <v>9.5</v>
       </c>
-      <c r="J2" s="4">
+      <c r="K2" s="4">
         <f>4+1+2+1+1+1</f>
         <v>10</v>
       </c>
-      <c r="K2" s="4">
+      <c r="L2" s="4">
         <v>2</v>
       </c>
-      <c r="L2" s="4">
-        <f>SUM(H2:K2)*2</f>
-        <v>49</v>
-      </c>
-      <c r="N2" s="4">
-        <f t="shared" ref="N2:N7" si="0">SUM(B2:E2)+L2</f>
-        <v>128</v>
+      <c r="M2" s="4">
+        <f>SUM(H2:L2)*2</f>
+        <v>51</v>
       </c>
       <c r="O2" s="4">
-        <f>SUM(N2+N2*0.1)</f>
-        <v>140.80000000000001</v>
-      </c>
-      <c r="Q2" s="4">
-        <f>SUM(N2:N7)</f>
-        <v>243</v>
+        <f t="shared" ref="O2:O7" si="0">SUM(B2:E2)+M2</f>
+        <v>130</v>
+      </c>
+      <c r="P2" s="4">
+        <f>SUM(O2+O2*0.1)</f>
+        <v>143</v>
       </c>
       <c r="R2" s="4">
-        <f>SUM(Q2+Q2*0.1)</f>
-        <v>267.3</v>
+        <f>SUM(O2:O7)</f>
+        <v>259</v>
+      </c>
+      <c r="S2" s="4">
+        <f>SUM(R2+R2*0.1)</f>
+        <v>284.89999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -701,29 +711,30 @@
       <c r="H3" s="4">
         <v>6</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="4"/>
+      <c r="J3" s="4">
         <f>1+1+2+2</f>
         <v>6</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4">
+      <c r="K3" s="4"/>
+      <c r="L3" s="4">
         <f>4+2+2</f>
         <v>8</v>
       </c>
-      <c r="L3" s="4">
-        <f t="shared" ref="L3:L7" si="1">SUM(H3:K3)*2</f>
+      <c r="M3" s="4">
+        <f t="shared" ref="M3:M7" si="1">SUM(H3:L3)*2</f>
         <v>40</v>
       </c>
-      <c r="N3" s="4">
+      <c r="O3" s="4">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
-      <c r="O3" s="4">
-        <f t="shared" ref="O3:O7" si="2">SUM(N3+N3*0.1)</f>
+      <c r="P3" s="4">
+        <f t="shared" ref="P3:P6" si="2">SUM(O3+O3*0.1)</f>
         <v>80.3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -743,23 +754,26 @@
       <c r="H4" s="4">
         <v>4</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="4">
+        <v>7</v>
+      </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="4">
+      <c r="L4" s="4"/>
+      <c r="M4" s="4">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="N4" s="4">
+        <v>22</v>
+      </c>
+      <c r="O4" s="4">
         <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="O4" s="4">
+        <v>33</v>
+      </c>
+      <c r="P4" s="4">
         <f t="shared" si="2"/>
-        <v>20.9</v>
+        <v>36.299999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -776,20 +790,21 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="4">
+      <c r="L5" s="4"/>
+      <c r="M5" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N5" s="4">
+      <c r="O5" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="O5" s="4">
+      <c r="P5" s="4">
         <f t="shared" si="2"/>
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -804,20 +819,21 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="4">
+      <c r="L6" s="4"/>
+      <c r="M6" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N6" s="4">
+      <c r="O6" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="O6" s="4">
+      <c r="P6" s="4">
         <f t="shared" si="2"/>
         <v>18.7</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -832,20 +848,21 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="4">
+      <c r="L7" s="4"/>
+      <c r="M7" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N7" s="4">
+      <c r="O7" s="4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="O7" s="4">
-        <f>SUM(N7+N7*0.1)</f>
+      <c r="P7" s="4">
+        <f>SUM(O7+O7*0.1)</f>
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
@@ -861,7 +878,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="N2:N3" formulaRange="1"/>
+    <ignoredError sqref="O2:O3" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added should to BOM
</commit_message>
<xml_diff>
--- a/Documents/TB_BOM.xlsx
+++ b/Documents/TB_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Win\Documents\GitHub\UofSC-ASME-Tiger-Burn-Design-2025\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6573D5E0-20B7-4022-BA13-464722788A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D3C34A-D728-4CD8-A926-F00C645BAA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5016" yWindow="1644" windowWidth="23040" windowHeight="12216" xr2:uid="{5E11D219-2DD1-4F5F-BD59-159B1B8915B2}"/>
   </bookViews>
@@ -559,7 +559,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>